<commit_message>
making the history page dynamic
</commit_message>
<xml_diff>
--- a/cchs_football_stats/example files/PlaylistData_2022-05-21 (1).xlsx
+++ b/cchs_football_stats/example files/PlaylistData_2022-05-21 (1).xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\OneDrive\Documents\GitHub\CCHS-Football-Stats\cchs_football_stats\example files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{000612D3-4F33-49BB-A462-A2E1034F0106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6174A69C-B984-412B-8792-332C8BD1B23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1231,6 +1243,34 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>